<commit_message>
Finalized sprint 1, started sprint 2
</commit_message>
<xml_diff>
--- a/project/Sprint01.xlsx
+++ b/project/Sprint01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\masters\cse551\CSE551\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmiele\Documents\Masters\CSE551\CSE551\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
   <si>
     <t xml:space="preserve">Product backlog item  </t>
   </si>
@@ -156,13 +156,17 @@
   </si>
   <si>
     <t>Totals</t>
+  </si>
+  <si>
+    <t>Team ended up catching the flu-like bug over the weekend and little work actually got done.
+Going to carry over objectives from this sprint to next sprint and do some weekend meetup time to catch up.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +237,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,8 +276,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -274,11 +290,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -342,9 +374,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -511,16 +548,16 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1705,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,19 +1829,19 @@
       </c>
       <c r="H2" s="25">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23.5</v>
       </c>
       <c r="I2" s="25">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>21.5</v>
       </c>
       <c r="J2" s="25">
         <f t="shared" si="0"/>
-        <v>23.5</v>
+        <v>22</v>
       </c>
       <c r="K2" s="25">
         <f t="shared" si="0"/>
-        <v>23.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1923,20 +1960,19 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H6" si="6">G5</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I6" si="7">H5</f>
-        <v>1</v>
+        <f t="shared" ref="I5:I6" si="6">H5</f>
+        <v>0.5</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J6" si="8">I5</f>
-        <v>1</v>
+        <f t="shared" ref="J5:J6" si="7">I5</f>
+        <v>0.5</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K6" si="9">J5</f>
-        <v>1</v>
+        <f t="shared" ref="K5:K6" si="8">J5</f>
+        <v>0.5</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -1972,19 +2008,19 @@
         <v>1</v>
       </c>
       <c r="H6">
+        <f t="shared" ref="H5:H6" si="9">G6</f>
+        <v>1</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="L6" t="s">
@@ -2067,16 +2103,15 @@
         <v>4</v>
       </c>
       <c r="I8">
-        <f t="shared" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -2197,12 +2232,11 @@
         <v>3</v>
       </c>
       <c r="J11">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K11">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2499,12 +2533,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A19:E23"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C18 C24">
       <formula1>"Peter, Daniela, Jennifer"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>